<commit_message>
Update CRONOGRAMA- SANTA ROSA.xlsx
</commit_message>
<xml_diff>
--- a/9.0 CRONOGRAMA/CRONOGRAMA- SANTA ROSA.xlsx
+++ b/9.0 CRONOGRAMA/CRONOGRAMA- SANTA ROSA.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ORFEI 751\Documents\GitHub\IOARR0005-SANTA-ROSA\9.0 CRONOGRAMA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositorioORFEI\IOARR0005-SANTA-ROSA\9.0 CRONOGRAMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$F$20</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -106,7 +106,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>OPTIMIZACION MEDIANTE COBERTURA DE LA LOSA DEPORTIVA MULTIUSO DE LA IEP N°54411 "ANDRES AVELINO CACERES",DISTRITO SANTA ROSA, PROVINCIA GRAU-REGION APURIMAC</t>
+      <t>OPTIMIZACION MEDIANTE COBERTURA DE LA LOSA DEPORTIVA MULTIUSO DE LA IEP N°54411 "ANDRES AVELINO CACERES - SANTA ROSA",DISTRITO SANTA ROSA, PROVINCIA GRAU-REGION APURIMAC</t>
     </r>
     <r>
       <rPr>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_ &quot;S/&quot;\ * #,##0.00_ ;_ &quot;S/&quot;\ * \-#,##0.00_ ;_ &quot;S/&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -804,21 +804,21 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="150" zoomScaleNormal="110" zoomScaleSheetLayoutView="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="1"/>
-    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
@@ -828,7 +828,7 @@
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
     </row>
-    <row r="2" spans="1:6" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
@@ -848,7 +848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -863,7 +863,7 @@
         <v>3524.03</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>18</v>
       </c>
@@ -873,7 +873,7 @@
       <c r="E4" s="32"/>
       <c r="F4" s="33"/>
     </row>
-    <row r="5" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -888,7 +888,7 @@
         <v>127623.44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -906,7 +906,7 @@
         <v>80547.539999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>19</v>
       </c>
@@ -921,7 +921,7 @@
         <v>16061.35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>15</v>
       </c>
@@ -936,7 +936,7 @@
         <v>7363.19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -951,7 +951,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -970,23 +970,25 @@
         <v>239119.55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="16">
-        <v>9668.3549999999996</v>
+        <f>F11/2</f>
+        <v>31508.89</v>
       </c>
       <c r="D11" s="16">
-        <v>9668.3549999999996</v>
+        <f>F11/2</f>
+        <v>31508.89</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="18">
         <v>63017.78</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>24961.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1022,7 +1024,7 @@
         <v>15464.06</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1037,7 +1039,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>17290.75</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -1062,11 +1064,11 @@
       </c>
       <c r="C16" s="20">
         <f>SUM(C10:C15)</f>
-        <v>205302.375</v>
+        <v>227142.91</v>
       </c>
       <c r="D16" s="20">
         <f>SUM(D10:D15)</f>
-        <v>93579.444999999992</v>
+        <v>115419.98</v>
       </c>
       <c r="E16" s="20">
         <f>SUM(E10:E15)</f>
@@ -1074,7 +1076,7 @@
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>12</v>
       </c>

</xml_diff>